<commit_message>
Added validation for ARDS Started COVID-19 showcase scenario and validation Added more outputs for some respiratory conditions scenarios
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/Scenarios/RespiratoryValidation.xlsx
+++ b/data/human/adult/validation/Scenarios/RespiratoryValidation.xlsx
@@ -1,47 +1,51 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse_Documentation\source\test\validation\Scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse_multiplex_ventilation\source\data\human\adult\validation\Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B8DD8E-E1C5-457F-86E1-A7C7E2882E6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59215B4A-3E9E-4312-A5E9-CCEBA9846650}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14055" yWindow="5250" windowWidth="30495" windowHeight="24645" tabRatio="643" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="915" yWindow="7395" windowWidth="24660" windowHeight="21360" tabRatio="643" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="21" r:id="rId1"/>
     <sheet name="AsthmaAttack" sheetId="32" r:id="rId2"/>
     <sheet name="COPD" sheetId="34" r:id="rId3"/>
-    <sheet name="LobarPneumonia" sheetId="35" r:id="rId4"/>
-    <sheet name="PulmonaryFibrosis" sheetId="47" r:id="rId5"/>
-    <sheet name="TensionPneumothorax" sheetId="44" r:id="rId6"/>
-    <sheet name="AirwayObstructionVaried" sheetId="16" r:id="rId7"/>
-    <sheet name="Bronchoconstriction" sheetId="23" r:id="rId8"/>
-    <sheet name="MainstemIntubation" sheetId="19" r:id="rId9"/>
-    <sheet name="EsophagealIntubation" sheetId="24" r:id="rId10"/>
-    <sheet name="Dyspnea" sheetId="45" r:id="rId11"/>
-    <sheet name="Supplemental Oxygen" sheetId="46" r:id="rId12"/>
+    <sheet name="ARDS" sheetId="49" r:id="rId4"/>
+    <sheet name="LobarPneumonia" sheetId="35" r:id="rId5"/>
+    <sheet name="PulmonaryFibrosis" sheetId="47" r:id="rId6"/>
+    <sheet name="TensionPneumothorax" sheetId="44" r:id="rId7"/>
+    <sheet name="AirwayObstructionVaried" sheetId="16" r:id="rId8"/>
+    <sheet name="Bronchoconstriction" sheetId="23" r:id="rId9"/>
+    <sheet name="MainstemIntubation" sheetId="19" r:id="rId10"/>
+    <sheet name="EsophagealIntubation" sheetId="24" r:id="rId11"/>
+    <sheet name="Dyspnea" sheetId="45" r:id="rId12"/>
+    <sheet name="Supplemental Oxygen" sheetId="46" r:id="rId13"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="6">AirwayObstructionVaried!#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="7">AirwayObstructionVaried!#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">ARDS!$B$1:$X$8</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">AsthmaAttack!$B$2:$Z$6</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="7">Bronchoconstriction!#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="8">Bronchoconstriction!#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">COPD!$B$2:$X$13</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="9">EsophagealIntubation!#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">LobarPneumonia!$B$2:$X$5</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="8">MainstemIntubation!#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Summary!$B$1:$J$17</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="10">EsophagealIntubation!#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">LobarPneumonia!$B$2:$X$5</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="9">MainstemIntubation!#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Summary!$B$1:$J$18</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -49,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1878" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1961" uniqueCount="278">
   <si>
     <t>Oxygen Saturation</t>
   </si>
@@ -829,6 +833,60 @@
   </si>
   <si>
     <t>Increase, Pulmonary Hypertension, &gt; 140 mm Hg @cite raghu2015pulmonary</t>
+  </si>
+  <si>
+    <t>ARDS Moderate</t>
+  </si>
+  <si>
+    <t>Moderate ARDS Severity = 0.6 Left Lung = 100% Right Lung  = 100%</t>
+  </si>
+  <si>
+    <t>Chronic condition</t>
+  </si>
+  <si>
+    <t>&lt;300 @cite mortelliti2002acute</t>
+  </si>
+  <si>
+    <t>Reduced @cite mortelliti2002acute</t>
+  </si>
+  <si>
+    <t>Normal or near normal @cite mortelliti2002acute</t>
+  </si>
+  <si>
+    <t>Tachypnea @cite mortelliti2002acute</t>
+  </si>
+  <si>
+    <t>Hypoxemia @cite radermacher2017fifty</t>
+  </si>
+  <si>
+    <t>&gt;20% @cite radermacher2017fifty</t>
+  </si>
+  <si>
+    <t>Increased @ cite mortelliti2002acute</t>
+  </si>
+  <si>
+    <t>Shunt Fraction</t>
+  </si>
+  <si>
+    <t>Tachycardia @cite mortelliti2002acute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Pulmonary Ventilation (L/min) </t>
+  </si>
+  <si>
+    <t>Hypoxia @cite mortelliti2002acute</t>
+  </si>
+  <si>
+    <t>ARDSModerateBothLungs</t>
+  </si>
+  <si>
+    <t>Moderate Acute Respiratory Distress Syndrome</t>
+  </si>
+  <si>
+    <t>Pulmonary Compliance (L/cmH2O)</t>
+  </si>
+  <si>
+    <t>Carrico Index [PaO2/FiO2] (mmHg)</t>
   </si>
 </sst>
 </file>
@@ -1460,7 +1518,7 @@
     <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1555,6 +1613,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="94">
@@ -1999,10 +2060,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2271,31 +2332,31 @@
         <v>49</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>32</v>
+        <v>274</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>194</v>
+        <v>275</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>101</v>
       </c>
       <c r="F8" s="28">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>104</v>
       </c>
       <c r="H8" s="29">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>105</v>
       </c>
       <c r="J8" s="30">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>102</v>
@@ -2306,25 +2367,25 @@
         <v>49</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>101</v>
       </c>
       <c r="F9" s="28">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>104</v>
       </c>
       <c r="H9" s="29">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>105</v>
@@ -2341,25 +2402,25 @@
         <v>49</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>101</v>
       </c>
       <c r="F10" s="28">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>104</v>
       </c>
       <c r="H10" s="29">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>105</v>
@@ -2376,19 +2437,19 @@
         <v>49</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>257</v>
+        <v>34</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>244</v>
+        <v>196</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>101</v>
       </c>
       <c r="F11" s="28">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>104</v>
@@ -2400,7 +2461,7 @@
         <v>105</v>
       </c>
       <c r="J11" s="30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>102</v>
@@ -2411,19 +2472,19 @@
         <v>49</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>45</v>
+        <v>257</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>47</v>
+        <v>244</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>101</v>
       </c>
       <c r="F12" s="28">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>104</v>
@@ -2446,19 +2507,19 @@
         <v>49</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>101</v>
       </c>
       <c r="F13" s="28">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>104</v>
@@ -2470,7 +2531,7 @@
         <v>105</v>
       </c>
       <c r="J13" s="30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>102</v>
@@ -2481,31 +2542,31 @@
         <v>49</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="8" t="s">
-        <v>197</v>
+      <c r="D14" s="27" t="s">
+        <v>48</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>101</v>
       </c>
       <c r="F14" s="28">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>104</v>
       </c>
       <c r="H14" s="29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>105</v>
       </c>
       <c r="J14" s="30">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K14" s="3" t="s">
         <v>102</v>
@@ -2516,19 +2577,19 @@
         <v>49</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>101</v>
       </c>
       <c r="F15" s="28">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>104</v>
@@ -2540,7 +2601,7 @@
         <v>105</v>
       </c>
       <c r="J15" s="30">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K15" s="3" t="s">
         <v>102</v>
@@ -2551,19 +2612,19 @@
         <v>49</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>212</v>
+        <v>16</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>101</v>
       </c>
       <c r="F16" s="28">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>104</v>
@@ -2575,7 +2636,7 @@
         <v>105</v>
       </c>
       <c r="J16" s="30">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K16" s="3" t="s">
         <v>102</v>
@@ -2586,19 +2647,19 @@
         <v>49</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>17</v>
+        <v>212</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>198</v>
+        <v>213</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>101</v>
       </c>
       <c r="F17" s="28">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>104</v>
@@ -2621,19 +2682,19 @@
         <v>49</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>256</v>
+        <v>17</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="27" t="s">
-        <v>211</v>
+      <c r="D18" s="8" t="s">
+        <v>198</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>101</v>
       </c>
       <c r="F18" s="28">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>104</v>
@@ -2656,19 +2717,19 @@
         <v>49</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>229</v>
+        <v>256</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D19" s="27" t="s">
-        <v>230</v>
+        <v>211</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>101</v>
       </c>
       <c r="F19" s="28">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>104</v>
@@ -2690,35 +2751,70 @@
       <c r="A20" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="26"/>
+      <c r="B20" s="26" t="s">
+        <v>229</v>
+      </c>
       <c r="C20" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>200</v>
+      <c r="D20" s="27" t="s">
+        <v>230</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>101</v>
       </c>
       <c r="F20" s="28">
-        <f>SUM(F3:F19)</f>
-        <v>241</v>
+        <v>3</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>104</v>
       </c>
       <c r="H20" s="29">
-        <f>SUM(H3:H19)</f>
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="I20" s="3" t="s">
         <v>105</v>
       </c>
       <c r="J20" s="30">
-        <f>SUM(J3:J19)</f>
+        <v>0</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="26"/>
+      <c r="C21" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F21" s="28">
+        <f>SUM(F3:F20)</f>
+        <v>250</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="H21" s="29">
+        <f>SUM(H3:H20)</f>
         <v>22</v>
       </c>
-      <c r="K20" s="3" t="s">
+      <c r="I21" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="J21" s="30">
+        <f>SUM(J3:J20)</f>
+        <v>22</v>
+      </c>
+      <c r="K21" s="3" t="s">
         <v>102</v>
       </c>
     </row>
@@ -2733,6 +2829,408 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:S6"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S6" sqref="A1:S6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2" style="14" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="2" style="14" customWidth="1"/>
+    <col min="4" max="4" width="30.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2" style="14" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2" style="14" customWidth="1"/>
+    <col min="8" max="8" width="22" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9" style="14" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20" style="2" customWidth="1"/>
+    <col min="21" max="21" width="9.140625" style="2"/>
+    <col min="22" max="22" width="13" style="2" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>238</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="7">
+        <v>60</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" s="7">
+        <v>180</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="L3" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="N3" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="P3" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="R3" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="7">
+        <v>180</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" s="7">
+        <v>480</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="P4" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="R4" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="7">
+        <v>480</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="7">
+        <v>600</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="L5" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="N5" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="P5" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="R5" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="7">
+        <v>600</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" s="7">
+        <v>900</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="N6" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="P6" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="R6" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="38" orientation="landscape" r:id="rId1"/>
+  <headerFooter scaleWithDoc="0">
+    <oddHeader>&amp;L&amp;A</oddHeader>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -3013,7 +3511,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:K8"/>
   <sheetViews>
@@ -3321,7 +3819,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:K14"/>
   <sheetViews>
@@ -4794,7 +5292,7 @@
   <dimension ref="A1:Y29"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Y4" sqref="A2:Y4"/>
+      <selection activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5374,14 +5872,342 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3EEE5A6-10C7-4039-9634-DA48737A2139}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:Y19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="W13" sqref="W13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="25.140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="26.42578125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="34.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="24.140625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="29.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="29.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.42578125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="29.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="29.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="29.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="29.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="29.5703125" style="2" customWidth="1"/>
+    <col min="25" max="25" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="V1" s="16"/>
+    </row>
+    <row r="2" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="V2" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="X2" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="V3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="X3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="8">
+        <v>120</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="P4" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="R4" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="T4" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="V4" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="X4" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="V5" s="17"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="V6" s="16"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="D8" s="1"/>
+      <c r="H8" s="33"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="D16" s="1"/>
+    </row>
+    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G19" s="33"/>
+    </row>
+  </sheetData>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="30" orientation="landscape" r:id="rId1"/>
+  <headerFooter scaleWithDoc="0">
+    <oddHeader>&amp;L&amp;A</oddHeader>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:Y36"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Y14" sqref="Y14"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6196,12 +7022,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Y4" sqref="A2:Y4"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I61" sqref="I61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6473,7 +7299,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:W19"/>
   <sheetViews>
@@ -7596,7 +8422,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -8113,7 +8939,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -8628,406 +9454,4 @@
     <oddHeader>&amp;L&amp;A</oddHeader>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:S6"/>
-  <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S6" sqref="A1:S6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="2" style="14" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="2" style="14" customWidth="1"/>
-    <col min="4" max="4" width="30.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2" style="14" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2" style="14" customWidth="1"/>
-    <col min="8" max="8" width="22" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9" style="14" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20" style="2" customWidth="1"/>
-    <col min="21" max="21" width="9.140625" style="2"/>
-    <col min="22" max="22" width="13" style="2" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>238</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H1" s="22" t="s">
-        <v>168</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="R2" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F3" s="7">
-        <v>60</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H3" s="7">
-        <v>180</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="L3" s="23" t="s">
-        <v>184</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="N3" s="23" t="s">
-        <v>184</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="P3" s="23" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="R3" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F4" s="7">
-        <v>180</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H4" s="7">
-        <v>480</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="N4" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="P4" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="R4" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F5" s="7">
-        <v>480</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H5" s="7">
-        <v>600</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="L5" s="23" t="s">
-        <v>184</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="N5" s="23" t="s">
-        <v>184</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="P5" s="23" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q5" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="R5" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="S5" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6" s="7">
-        <v>600</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H6" s="7">
-        <v>900</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="L6" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="N6" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="P6" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="Q6" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="R6" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="S6" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="38" orientation="landscape" r:id="rId1"/>
-  <headerFooter scaleWithDoc="0">
-    <oddHeader>&amp;L&amp;A</oddHeader>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Documentation updates. Updated Respiratory and Mechanical Ventilator plots. Updated publication link. Small tweaks to methodology reports.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/Scenarios/RespiratoryValidation.xlsx
+++ b/data/human/adult/validation/Scenarios/RespiratoryValidation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse_multiplex_ventilation\source\data\human\adult\validation\Scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse\source-documentation-3.2_Release\data\human\adult\validation\Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59215B4A-3E9E-4312-A5E9-CCEBA9846650}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95577ED-CB6E-4B10-93C0-C8EBBC003EB2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="915" yWindow="7395" windowWidth="24660" windowHeight="21360" tabRatio="643" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23145" yWindow="8835" windowWidth="31575" windowHeight="19245" tabRatio="643" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="21" r:id="rId1"/>
@@ -2062,8 +2062,8 @@
   </sheetPr>
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2414,13 +2414,13 @@
         <v>101</v>
       </c>
       <c r="F10" s="28">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>104</v>
       </c>
       <c r="H10" s="29">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>105</v>
@@ -2798,14 +2798,14 @@
       </c>
       <c r="F21" s="28">
         <f>SUM(F3:F20)</f>
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>104</v>
       </c>
       <c r="H21" s="29">
         <f>SUM(H3:H20)</f>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I21" s="3" t="s">
         <v>105</v>
@@ -4185,8 +4185,8 @@
   </sheetPr>
   <dimension ref="A1:AA37"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AA17" sqref="A14:AA17"/>
+    <sheetView topLeftCell="P1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5878,7 +5878,7 @@
   </sheetPr>
   <dimension ref="A1:Y19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
@@ -6207,7 +6207,7 @@
   <dimension ref="A1:Y36"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A7" sqref="A7:Y9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6671,9 +6671,9 @@
         <v>86</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="L9" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="L9" s="10" t="s">
         <v>114</v>
       </c>
       <c r="M9" s="3" t="s">
@@ -6689,9 +6689,9 @@
         <v>116</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="R9" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="R9" s="10" t="s">
         <v>117</v>
       </c>
       <c r="S9" s="3" t="s">
@@ -7026,7 +7026,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="K1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="I61" sqref="I61"/>
     </sheetView>
   </sheetViews>
@@ -8430,7 +8430,7 @@
   <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S8" sqref="A1:S8"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add Hemothorax validation (again)
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/Scenarios/RespiratoryValidation.xlsx
+++ b/data/human/adult/validation/Scenarios/RespiratoryValidation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse\4.x\source\data\human\adult\validation\Scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Pulse\biomojo\engine\data\human\adult\validation\Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB7C6E81-7D18-4B2E-B89F-BC1BD8D53349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB0BCB38-C815-4970-935A-DFD9D5BE9C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9525" yWindow="1950" windowWidth="44520" windowHeight="23535" tabRatio="643" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="48480" yWindow="-120" windowWidth="57840" windowHeight="31920" tabRatio="643" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="21" r:id="rId1"/>
@@ -20,22 +20,23 @@
     <sheet name="LobarPneumonia" sheetId="35" r:id="rId5"/>
     <sheet name="PulmonaryFibrosis" sheetId="47" r:id="rId6"/>
     <sheet name="TensionPneumothorax" sheetId="44" r:id="rId7"/>
-    <sheet name="AirwayObstructionVaried" sheetId="16" r:id="rId8"/>
-    <sheet name="Bronchoconstriction" sheetId="23" r:id="rId9"/>
-    <sheet name="MainstemIntubation" sheetId="19" r:id="rId10"/>
-    <sheet name="EsophagealIntubation" sheetId="24" r:id="rId11"/>
-    <sheet name="Dyspnea" sheetId="45" r:id="rId12"/>
-    <sheet name="Supplemental Oxygen" sheetId="46" r:id="rId13"/>
+    <sheet name="Hemothorax" sheetId="50" r:id="rId8"/>
+    <sheet name="AirwayObstructionVaried" sheetId="16" r:id="rId9"/>
+    <sheet name="Bronchoconstriction" sheetId="23" r:id="rId10"/>
+    <sheet name="MainstemIntubation" sheetId="19" r:id="rId11"/>
+    <sheet name="EsophagealIntubation" sheetId="24" r:id="rId12"/>
+    <sheet name="Dyspnea" sheetId="45" r:id="rId13"/>
+    <sheet name="Supplemental Oxygen" sheetId="46" r:id="rId14"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="7">AirwayObstructionVaried!#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="8">AirwayObstructionVaried!#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">ARDS!$B$1:$X$8</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">AsthmaAttack!$B$2:$Z$6</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="8">Bronchoconstriction!#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="9">Bronchoconstriction!#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">COPD!$B$2:$X$13</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="10">EsophagealIntubation!#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="11">EsophagealIntubation!#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">LobarPneumonia!$B$2:$X$5</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="9">MainstemIntubation!#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="10">MainstemIntubation!#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Summary!$B$1:$J$18</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1991" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2143" uniqueCount="317">
   <si>
     <t>Oxygen Saturation</t>
   </si>
@@ -911,6 +912,99 @@
   </si>
   <si>
     <t>Tension Pneumothorax;  Closed,   severity = 1.0</t>
+  </si>
+  <si>
+    <t>HemothoraxVaried</t>
+  </si>
+  <si>
+    <t>Blood Volume (mL)</t>
+  </si>
+  <si>
+    <t>Left Lung Volume (mL)</t>
+  </si>
+  <si>
+    <t>Pulse Pressure (mmHg)</t>
+  </si>
+  <si>
+    <t>Hemothorax: severity = 0.0</t>
+  </si>
+  <si>
+    <t>Hemothorax: flow rate = 0.1 mL/s</t>
+  </si>
+  <si>
+    <t>Represents a minimal traumatic hemothorax on the left lung side.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">~72 reduction from initial @cite zeiler2020hemothorax </t>
+  </si>
+  <si>
+    <t>Decrease  @cite dogrul2020blunt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Increase @cite gomez2022hemothorax </t>
+  </si>
+  <si>
+    <t>Increase @cite dogrul2020blunt</t>
+  </si>
+  <si>
+    <t>Decrease @cite dogrul2020blunt</t>
+  </si>
+  <si>
+    <t>Decrease @cite gomez2022hemothorax</t>
+  </si>
+  <si>
+    <t>Hemothorax: flow rate = 0.5 mL/s</t>
+  </si>
+  <si>
+    <t>Represents a medium traumatic hemothorax on the left lung side.</t>
+  </si>
+  <si>
+    <t>~432 reduction from initial @cite zeiler2020hemothorax</t>
+  </si>
+  <si>
+    <t>Hemothorax: flow rate = 1.0 mL/s</t>
+  </si>
+  <si>
+    <t>Represents a massive traumatic hemothorax on the left lung side. Should lead to full collapse.</t>
+  </si>
+  <si>
+    <t>~1500  reduction from initial @cite zeiler2020hemothorax</t>
+  </si>
+  <si>
+    <t>Decrease (atelectasis) @cite dogrul2020blunt</t>
+  </si>
+  <si>
+    <t>Increase (tachypnea)  @cite gomez2022hemothorax</t>
+  </si>
+  <si>
+    <t>Increase (tachycardia) @cite dogrul2020blunt</t>
+  </si>
+  <si>
+    <t>Decrease (hypotension) @cite dogrul2020blunt</t>
+  </si>
+  <si>
+    <t>Decrease (narrow) @cite gomez2022hemothorax</t>
+  </si>
+  <si>
+    <t>Decrease (hypoxia)  @cite gomez2022hemothorax</t>
+  </si>
+  <si>
+    <t>Hemothorax: flow rate = 0.0 mL/s; Apply Tube Thoracostomy</t>
+  </si>
+  <si>
+    <t>Stop the hemothorax and apply a tube thoracostomy on the left side of the chest to suck blood out of the pleural space.</t>
+  </si>
+  <si>
+    <t>No Change or slight increase</t>
+  </si>
+  <si>
+    <t>Returning toward normal @cite dogrul2020blunt</t>
+  </si>
+  <si>
+    <t>Returning toward normal @cite gomez2022hemothorax</t>
+  </si>
+  <si>
+    <t>Returning toward normal  @cite gomez2022hemothorax</t>
   </si>
 </sst>
 </file>
@@ -1542,7 +1636,7 @@
     <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1618,6 +1712,25 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="94">
@@ -2068,23 +2181,23 @@
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="57.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.54296875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="12" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>49</v>
       </c>
@@ -2119,7 +2232,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>49</v>
       </c>
@@ -2154,7 +2267,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>49</v>
       </c>
@@ -2189,7 +2302,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>49</v>
       </c>
@@ -2224,7 +2337,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>49</v>
       </c>
@@ -2259,7 +2372,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>49</v>
       </c>
@@ -2294,7 +2407,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>49</v>
       </c>
@@ -2329,7 +2442,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>49</v>
       </c>
@@ -2364,7 +2477,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>49</v>
       </c>
@@ -2399,7 +2512,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>49</v>
       </c>
@@ -2434,7 +2547,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>49</v>
       </c>
@@ -2469,7 +2582,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>49</v>
       </c>
@@ -2504,7 +2617,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>49</v>
       </c>
@@ -2539,7 +2652,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>49</v>
       </c>
@@ -2574,7 +2687,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>49</v>
       </c>
@@ -2609,7 +2722,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>49</v>
       </c>
@@ -2644,7 +2757,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>49</v>
       </c>
@@ -2679,7 +2792,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>49</v>
       </c>
@@ -2714,7 +2827,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>49</v>
       </c>
@@ -2749,7 +2862,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>49</v>
       </c>
@@ -2784,7 +2897,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>49</v>
       </c>
@@ -2831,6 +2944,523 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:S8"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S8" sqref="A1:S8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="2" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2" style="1" customWidth="1"/>
+    <col min="4" max="4" width="26" style="1" customWidth="1"/>
+    <col min="5" max="5" width="2" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2" style="1" customWidth="1"/>
+    <col min="8" max="8" width="22" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.1796875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="87" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="5">
+        <v>30</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" s="1">
+        <v>180</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="L3" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N3" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P3" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="R3" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="5">
+        <v>210</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" s="5">
+        <v>300</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="R4" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="5">
+        <v>510</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="1">
+        <v>180</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="N5" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P5" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="R5" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="5">
+        <v>690</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" s="5">
+        <v>300</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="5">
+        <v>990</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" s="1">
+        <v>180</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J7" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="L7" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="N7" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P7" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="R7" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="5">
+        <v>1170</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" s="5">
+        <v>500</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="R8" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="39" orientation="landscape" r:id="rId1"/>
+  <headerFooter scaleWithDoc="0">
+    <oddHeader>&amp;L&amp;A</oddHeader>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -2841,34 +3471,34 @@
       <selection activeCell="S6" sqref="A1:S6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.26953125" style="1" customWidth="1"/>
     <col min="3" max="3" width="2" style="1" customWidth="1"/>
-    <col min="4" max="4" width="30.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2" style="1" customWidth="1"/>
     <col min="8" max="8" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="20" style="1" customWidth="1"/>
-    <col min="21" max="21" width="9.140625" style="1"/>
+    <col min="21" max="21" width="9.1796875" style="1"/>
     <col min="22" max="22" width="13" style="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="1"/>
+    <col min="23" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>49</v>
       </c>
@@ -2927,7 +3557,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>49</v>
       </c>
@@ -2986,7 +3616,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>49</v>
       </c>
@@ -3045,7 +3675,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>49</v>
       </c>
@@ -3104,7 +3734,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>49</v>
       </c>
@@ -3163,7 +3793,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>49</v>
       </c>
@@ -3232,7 +3862,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -3243,31 +3873,31 @@
       <selection activeCell="S4" sqref="A1:S4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="1"/>
+    <col min="20" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>49</v>
       </c>
@@ -3326,7 +3956,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>49</v>
       </c>
@@ -3385,7 +4015,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>49</v>
       </c>
@@ -3444,7 +4074,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>49</v>
       </c>
@@ -3513,7 +4143,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:K8"/>
   <sheetViews>
@@ -3521,22 +4151,22 @@
       <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>49</v>
       </c>
@@ -3571,7 +4201,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>49</v>
       </c>
@@ -3606,7 +4236,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>49</v>
       </c>
@@ -3641,7 +4271,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>49</v>
       </c>
@@ -3676,7 +4306,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>49</v>
       </c>
@@ -3711,7 +4341,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>49</v>
       </c>
@@ -3746,7 +4376,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>49</v>
       </c>
@@ -3781,7 +4411,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>49</v>
       </c>
@@ -3821,7 +4451,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:K14"/>
   <sheetViews>
@@ -3829,27 +4459,27 @@
       <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
     <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.7265625" customWidth="1"/>
     <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>49</v>
       </c>
@@ -3884,7 +4514,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>49</v>
       </c>
@@ -3919,7 +4549,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>49</v>
       </c>
@@ -3954,12 +4584,12 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>49</v>
       </c>
@@ -3994,7 +4624,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>49</v>
       </c>
@@ -4029,7 +4659,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>49</v>
       </c>
@@ -4064,12 +4694,12 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>49</v>
       </c>
@@ -4104,7 +4734,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>49</v>
       </c>
@@ -4139,7 +4769,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>49</v>
       </c>
@@ -4190,44 +4820,44 @@
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="29" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="33.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="30.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="30.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="32.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="30.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="33.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="33.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="30.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="30.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="32.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="30.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="16384" width="9.140625" style="1"/>
+    <col min="28" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:27" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>49</v>
       </c>
@@ -4310,7 +4940,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>49</v>
       </c>
@@ -4393,7 +5023,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>49</v>
       </c>
@@ -4474,7 +5104,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>49</v>
       </c>
@@ -4555,12 +5185,12 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>49</v>
       </c>
@@ -4643,7 +5273,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>49</v>
       </c>
@@ -4726,7 +5356,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" ht="58" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>49</v>
       </c>
@@ -4807,7 +5437,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>49</v>
       </c>
@@ -4888,12 +5518,12 @@
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>49</v>
       </c>
@@ -4976,7 +5606,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>49</v>
       </c>
@@ -5059,7 +5689,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:27" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" ht="58" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>49</v>
       </c>
@@ -5140,7 +5770,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>49</v>
       </c>
@@ -5221,58 +5851,58 @@
         <v>102</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.35">
       <c r="J20"/>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.35">
       <c r="J21"/>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.35">
       <c r="J22"/>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.35">
       <c r="J23"/>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.35">
       <c r="J24"/>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.35">
       <c r="J25"/>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.35">
       <c r="J26"/>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.35">
       <c r="J27"/>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.35">
       <c r="J28"/>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.35">
       <c r="J29"/>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.35">
       <c r="J30"/>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.35">
       <c r="J31"/>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.35">
       <c r="J32"/>
     </row>
-    <row r="33" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J33"/>
     </row>
-    <row r="34" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J34"/>
     </row>
-    <row r="35" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J35"/>
     </row>
-    <row r="36" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J36"/>
     </row>
-    <row r="37" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J37"/>
     </row>
   </sheetData>
@@ -5296,42 +5926,42 @@
       <selection activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="9.140625" style="1"/>
+    <col min="26" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>49</v>
       </c>
@@ -5408,7 +6038,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>49</v>
       </c>
@@ -5485,7 +6115,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="150" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>49</v>
       </c>
@@ -5562,16 +6192,16 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="V5" s="11"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>53</v>
       </c>
       <c r="V6" s="12"/>
     </row>
-    <row r="7" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>49</v>
       </c>
@@ -5648,7 +6278,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>49</v>
       </c>
@@ -5725,7 +6355,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>49</v>
       </c>
@@ -5800,66 +6430,66 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
       <c r="V10" s="11"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
       <c r="V11" s="12"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
       <c r="D12"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
       <c r="D13"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
       <c r="D14"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
       <c r="D15"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
       <c r="D16"/>
     </row>
-    <row r="17" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D17"/>
     </row>
-    <row r="18" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D18"/>
     </row>
-    <row r="19" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D19"/>
     </row>
-    <row r="20" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D20"/>
     </row>
-    <row r="21" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D21"/>
     </row>
-    <row r="22" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D22"/>
     </row>
-    <row r="23" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D23"/>
     </row>
-    <row r="24" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D24"/>
       <c r="J24"/>
     </row>
-    <row r="25" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D25"/>
       <c r="J25"/>
     </row>
-    <row r="26" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D26"/>
     </row>
-    <row r="27" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D27"/>
     </row>
-    <row r="28" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D28"/>
     </row>
-    <row r="29" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D29"/>
     </row>
   </sheetData>
@@ -5883,43 +6513,43 @@
       <selection activeCell="X16" sqref="X16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="25.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="26.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="34.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="24.140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.5703125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.42578125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.54296875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="25.1796875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="26.453125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="34.7265625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="24.1796875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.54296875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.453125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="29.5703125" style="1" customWidth="1"/>
+    <col min="23" max="23" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="29.54296875" style="1" customWidth="1"/>
     <col min="25" max="25" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="9.140625" style="1"/>
+    <col min="26" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>256</v>
       </c>
       <c r="V1" s="12"/>
     </row>
-    <row r="2" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>49</v>
       </c>
@@ -5996,7 +6626,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>49</v>
       </c>
@@ -6073,7 +6703,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>49</v>
       </c>
@@ -6150,44 +6780,44 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="V5" s="11"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="V6" s="12"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
       <c r="D7"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
       <c r="D8"/>
       <c r="H8" s="25"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
       <c r="D9"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
       <c r="D10"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
       <c r="D11"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
       <c r="D12"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
       <c r="D13"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
       <c r="D14"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
       <c r="D15"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
       <c r="D16"/>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G19" s="25"/>
     </row>
   </sheetData>
@@ -6211,42 +6841,42 @@
       <selection activeCell="A7" sqref="A7:Y9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="30.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="30.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="29.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="29.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="9.140625" style="1"/>
+    <col min="26" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>49</v>
       </c>
@@ -6323,7 +6953,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>49</v>
       </c>
@@ -6400,7 +7030,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="87" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>49</v>
       </c>
@@ -6477,15 +7107,15 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="Q5" s="15"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>49</v>
       </c>
@@ -6562,7 +7192,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>49</v>
       </c>
@@ -6639,7 +7269,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="87" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>49</v>
       </c>
@@ -6716,12 +7346,12 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>49</v>
       </c>
@@ -6798,7 +7428,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>49</v>
       </c>
@@ -6875,7 +7505,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="90" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" ht="87" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>49</v>
       </c>
@@ -6952,64 +7582,64 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H17"/>
     </row>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H18"/>
     </row>
-    <row r="19" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H19"/>
     </row>
-    <row r="20" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H20"/>
     </row>
-    <row r="21" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H21"/>
     </row>
-    <row r="22" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H22"/>
     </row>
-    <row r="23" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H23"/>
     </row>
-    <row r="24" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H24"/>
     </row>
-    <row r="25" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H25"/>
     </row>
-    <row r="26" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H26"/>
     </row>
-    <row r="27" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H27"/>
     </row>
-    <row r="28" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H28"/>
     </row>
-    <row r="29" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H29"/>
     </row>
-    <row r="30" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H30"/>
     </row>
-    <row r="31" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H31"/>
     </row>
-    <row r="32" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H32"/>
     </row>
-    <row r="33" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H33"/>
     </row>
-    <row r="34" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H34"/>
     </row>
-    <row r="35" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H35"/>
     </row>
-    <row r="36" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H36"/>
     </row>
   </sheetData>
@@ -7030,40 +7660,40 @@
       <selection activeCell="I61" sqref="I61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.26953125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="33.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="32.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.7265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="33.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="33.81640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="26.7265625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="33.1796875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="23" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="33.81640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>49</v>
       </c>
@@ -7140,7 +7770,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>49</v>
       </c>
@@ -7217,7 +7847,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>49</v>
       </c>
@@ -7303,46 +7933,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Y18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.5703125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.54296875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="33.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="33.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="33.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="33.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="33.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="33.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="9.140625" style="1"/>
+    <col min="25" max="25" width="9.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>49</v>
       </c>
@@ -7419,7 +8049,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>49</v>
       </c>
@@ -7496,7 +8126,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>49</v>
       </c>
@@ -7573,7 +8203,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>49</v>
       </c>
@@ -7650,7 +8280,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>49</v>
       </c>
@@ -7727,7 +8357,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>49</v>
       </c>
@@ -7804,7 +8434,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>49</v>
       </c>
@@ -7881,7 +8511,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>49</v>
       </c>
@@ -7958,12 +8588,12 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B11" s="19" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>49</v>
       </c>
@@ -8040,7 +8670,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>49</v>
       </c>
@@ -8117,7 +8747,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>49</v>
       </c>
@@ -8194,7 +8824,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="58" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>49</v>
       </c>
@@ -8271,7 +8901,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>49</v>
       </c>
@@ -8348,7 +8978,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" ht="58" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>49</v>
       </c>
@@ -8425,7 +9055,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>49</v>
       </c>
@@ -8509,6 +9139,557 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC2E4031-F2A3-4C30-8EF1-DCE54FAB3A4E}">
+  <dimension ref="A1:W8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X19" sqref="X19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="1.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.26953125" customWidth="1"/>
+    <col min="4" max="4" width="47.1796875" customWidth="1"/>
+    <col min="10" max="10" width="25.81640625" customWidth="1"/>
+    <col min="12" max="12" width="27.36328125" customWidth="1"/>
+    <col min="14" max="14" width="34.6328125" customWidth="1"/>
+    <col min="16" max="16" width="26.08984375" customWidth="1"/>
+    <col min="18" max="18" width="31.7265625" customWidth="1"/>
+    <col min="20" max="20" width="24.7265625" customWidth="1"/>
+    <col min="22" max="22" width="22.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A1" s="26"/>
+      <c r="B1" s="27" t="s">
+        <v>286</v>
+      </c>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+    </row>
+    <row r="2" spans="1:23" ht="58" x14ac:dyDescent="0.35">
+      <c r="A2" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>231</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="J2" s="29" t="s">
+        <v>287</v>
+      </c>
+      <c r="K2" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="L2" s="29" t="s">
+        <v>288</v>
+      </c>
+      <c r="M2" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="N2" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="O2" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="P2" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q2" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="R2" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="S2" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="T2" s="29" t="s">
+        <v>289</v>
+      </c>
+      <c r="U2" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="V2" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="W2" s="28" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A3" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="J3" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="K3" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="L3" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="M3" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="N3" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="O3" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="P3" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q3" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="R3" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="S3" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="T3" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="U3" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="V3" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="W3" s="28" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>290</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>236</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="30">
+        <v>30</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" s="30">
+        <v>60</v>
+      </c>
+      <c r="I4" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="J4" s="31" t="s">
+        <v>200</v>
+      </c>
+      <c r="K4" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="L4" s="31" t="s">
+        <v>200</v>
+      </c>
+      <c r="M4" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="N4" s="31" t="s">
+        <v>200</v>
+      </c>
+      <c r="O4" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="P4" s="31" t="s">
+        <v>200</v>
+      </c>
+      <c r="Q4" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="R4" s="31" t="s">
+        <v>200</v>
+      </c>
+      <c r="S4" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="T4" s="31" t="s">
+        <v>200</v>
+      </c>
+      <c r="U4" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="V4" s="31" t="s">
+        <v>200</v>
+      </c>
+      <c r="W4" s="28" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>291</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>292</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="30">
+        <v>60</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="30">
+        <v>780</v>
+      </c>
+      <c r="I5" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="J5" s="31" t="s">
+        <v>293</v>
+      </c>
+      <c r="K5" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="L5" s="31" t="s">
+        <v>294</v>
+      </c>
+      <c r="M5" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="N5" s="31" t="s">
+        <v>295</v>
+      </c>
+      <c r="O5" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="P5" s="31" t="s">
+        <v>296</v>
+      </c>
+      <c r="Q5" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="R5" s="32" t="s">
+        <v>297</v>
+      </c>
+      <c r="S5" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="T5" s="31" t="s">
+        <v>298</v>
+      </c>
+      <c r="U5" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="V5" s="32" t="s">
+        <v>298</v>
+      </c>
+      <c r="W5" s="28" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>299</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>300</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="30">
+        <v>780</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" s="30">
+        <v>1500</v>
+      </c>
+      <c r="I6" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="J6" s="31" t="s">
+        <v>301</v>
+      </c>
+      <c r="K6" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="L6" s="31" t="s">
+        <v>294</v>
+      </c>
+      <c r="M6" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="N6" s="31" t="s">
+        <v>295</v>
+      </c>
+      <c r="O6" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="P6" s="31" t="s">
+        <v>296</v>
+      </c>
+      <c r="Q6" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="R6" s="32" t="s">
+        <v>297</v>
+      </c>
+      <c r="S6" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="T6" s="31" t="s">
+        <v>298</v>
+      </c>
+      <c r="U6" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="V6" s="31" t="s">
+        <v>298</v>
+      </c>
+      <c r="W6" s="28" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>302</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>303</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="30">
+        <v>1500</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" s="30">
+        <v>2580</v>
+      </c>
+      <c r="I7" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="J7" s="31" t="s">
+        <v>304</v>
+      </c>
+      <c r="K7" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="L7" s="31" t="s">
+        <v>305</v>
+      </c>
+      <c r="M7" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="N7" s="31" t="s">
+        <v>306</v>
+      </c>
+      <c r="O7" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="P7" s="31" t="s">
+        <v>307</v>
+      </c>
+      <c r="Q7" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="R7" s="31" t="s">
+        <v>308</v>
+      </c>
+      <c r="S7" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="T7" s="31" t="s">
+        <v>309</v>
+      </c>
+      <c r="U7" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="V7" s="31" t="s">
+        <v>310</v>
+      </c>
+      <c r="W7" s="28" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>311</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>312</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="30">
+        <v>2580</v>
+      </c>
+      <c r="G8" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" s="30">
+        <v>4020</v>
+      </c>
+      <c r="I8" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="J8" s="31" t="s">
+        <v>313</v>
+      </c>
+      <c r="K8" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="L8" s="31" t="s">
+        <v>314</v>
+      </c>
+      <c r="M8" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="N8" s="31" t="s">
+        <v>315</v>
+      </c>
+      <c r="O8" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="P8" s="31" t="s">
+        <v>314</v>
+      </c>
+      <c r="Q8" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="R8" s="31" t="s">
+        <v>314</v>
+      </c>
+      <c r="S8" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="T8" s="31" t="s">
+        <v>315</v>
+      </c>
+      <c r="U8" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="V8" s="31" t="s">
+        <v>316</v>
+      </c>
+      <c r="W8" s="28" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -8519,31 +9700,31 @@
       <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="1"/>
+    <col min="20" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>49</v>
       </c>
@@ -8602,7 +9783,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>49</v>
       </c>
@@ -8661,7 +9842,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="105" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>49</v>
       </c>
@@ -8720,7 +9901,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>49</v>
       </c>
@@ -8779,7 +9960,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="87" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>49</v>
       </c>
@@ -8838,7 +10019,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>49</v>
       </c>
@@ -8897,7 +10078,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="87" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>49</v>
       </c>
@@ -8956,7 +10137,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>49</v>
       </c>
@@ -9023,521 +10204,4 @@
     <oddHeader>&amp;L&amp;A</oddHeader>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:S8"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S8" sqref="A1:S8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="2" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2" style="1" customWidth="1"/>
-    <col min="4" max="4" width="26" style="1" customWidth="1"/>
-    <col min="5" max="5" width="2" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2" style="1" customWidth="1"/>
-    <col min="8" max="8" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>234</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>164</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="90" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F3" s="5">
-        <v>30</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H3" s="1">
-        <v>180</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="J3" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="L3" s="18" t="s">
-        <v>176</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="N3" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="P3" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="R3" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F4" s="5">
-        <v>210</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H4" s="5">
-        <v>300</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="P4" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="R4" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F5" s="5">
-        <v>510</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H5" s="1">
-        <v>180</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="J5" s="17" t="s">
-        <v>155</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="L5" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="N5" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="P5" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="R5" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6" s="5">
-        <v>690</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H6" s="5">
-        <v>300</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="P6" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="R6" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="S6" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" s="5">
-        <v>990</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H7" s="1">
-        <v>180</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="J7" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="L7" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="N7" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="P7" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="R7" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="S7" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F8" s="5">
-        <v>1170</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H8" s="5">
-        <v>500</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="L8" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="N8" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="P8" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="Q8" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="R8" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="S8" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="39" orientation="landscape" r:id="rId1"/>
-  <headerFooter scaleWithDoc="0">
-    <oddHeader>&amp;L&amp;A</oddHeader>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added a bronchoconstriction death scenario.  Updated death scenario timing.  Updated airway obstruction and asthma to better meet validation.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/Scenarios/RespiratoryValidation.xlsx
+++ b/data/human/adult/validation/Scenarios/RespiratoryValidation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse\documentation\source\data\human\adult\validation\Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{972BDD08-427C-4ACB-8B7F-94EE64DEE5A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27555881-198A-40F6-BB1E-B04399C13B45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="285" yWindow="7725" windowWidth="56895" windowHeight="22365" tabRatio="643" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="32040" tabRatio="643" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="21" r:id="rId1"/>
@@ -2140,7 +2140,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2287,13 +2287,13 @@
         <v>101</v>
       </c>
       <c r="H4" s="21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>102</v>
       </c>
       <c r="J4" s="22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>99</v>
@@ -2316,19 +2316,19 @@
         <v>98</v>
       </c>
       <c r="F5" s="20">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>101</v>
       </c>
       <c r="H5" s="21">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>102</v>
       </c>
       <c r="J5" s="22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>99</v>
@@ -2910,21 +2910,21 @@
       </c>
       <c r="F22" s="20">
         <f>SUM(F3:F21)</f>
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>101</v>
       </c>
       <c r="H22" s="21">
         <f>SUM(H3:H21)</f>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>102</v>
       </c>
       <c r="J22" s="22">
         <f>SUM(J3:J21)</f>
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>99</v>
@@ -4814,7 +4814,7 @@
   <dimension ref="A1:AA37"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U16" sqref="U16"/>
+      <selection activeCell="AA17" sqref="AA17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5395,9 +5395,9 @@
         <v>73</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="P10" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="P10" s="8" t="s">
         <v>74</v>
       </c>
       <c r="Q10" s="2" t="s">
@@ -5716,9 +5716,9 @@
         <v>70</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="L16" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="L16" s="6" t="s">
         <v>72</v>
       </c>
       <c r="M16" s="2" t="s">
@@ -5728,9 +5728,9 @@
         <v>73</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="P16" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="P16" s="7" t="s">
         <v>78</v>
       </c>
       <c r="Q16" s="2" t="s">
@@ -5740,21 +5740,21 @@
         <v>67</v>
       </c>
       <c r="S16" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="T16" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="U16" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="V16" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="W16" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="T16" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="U16" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="V16" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="W16" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="X16" s="7" t="s">
+      <c r="X16" s="8" t="s">
         <v>66</v>
       </c>
       <c r="Y16" s="2" t="s">

</xml_diff>